<commit_message>
Not really sure what happened
</commit_message>
<xml_diff>
--- a/7Z015 and 7Z030 pinout comparison.xlsx
+++ b/7Z015 and 7Z030 pinout comparison.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Z015 and Z030 pinout comparison" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -3462,7 +3462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M489"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -3537,7 +3537,7 @@
         <v>9</v>
       </c>
       <c r="G4" s="1" t="b">
-        <f>(B4=J4)</f>
+        <f t="shared" ref="G4:G67" si="0">(B4=J4)</f>
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -3573,7 +3573,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="1" t="b">
-        <f>(B5=J5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -3609,7 +3609,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="1" t="b">
-        <f>(B6=J6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -3645,7 +3645,7 @@
         <v>9</v>
       </c>
       <c r="G7" s="1" t="b">
-        <f>(B7=J7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -3681,7 +3681,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="1" t="b">
-        <f>(B8=J8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -3717,7 +3717,7 @@
         <v>9</v>
       </c>
       <c r="G9" s="1" t="b">
-        <f>(B9=J9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -3753,7 +3753,7 @@
         <v>9</v>
       </c>
       <c r="G10" s="1" t="b">
-        <f>(B10=J10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -3789,7 +3789,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="1" t="b">
-        <f>(B11=J11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -3825,7 +3825,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="1" t="b">
-        <f>(B12=J12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -3861,7 +3861,7 @@
         <v>9</v>
       </c>
       <c r="G13" s="1" t="b">
-        <f>(B13=J13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -3897,7 +3897,7 @@
         <v>9</v>
       </c>
       <c r="G14" s="1" t="b">
-        <f>(B14=J14)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -3933,7 +3933,7 @@
         <v>9</v>
       </c>
       <c r="G15" s="1" t="b">
-        <f>(B15=J15)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -3969,7 +3969,7 @@
         <v>9</v>
       </c>
       <c r="G16" s="1" t="b">
-        <f>(B16=J16)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -4005,7 +4005,7 @@
         <v>9</v>
       </c>
       <c r="G17" s="1" t="b">
-        <f>(B17=J17)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -4041,7 +4041,7 @@
         <v>9</v>
       </c>
       <c r="G18" s="1" t="b">
-        <f>(B18=J18)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -4077,7 +4077,7 @@
         <v>9</v>
       </c>
       <c r="G19" s="1" t="b">
-        <f>(B19=J19)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -4113,7 +4113,7 @@
         <v>9</v>
       </c>
       <c r="G20" s="1" t="b">
-        <f>(B20=J20)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I20" s="1" t="s">
@@ -4149,7 +4149,7 @@
         <v>9</v>
       </c>
       <c r="G21" s="1" t="b">
-        <f>(B21=J21)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I21" s="1" t="s">
@@ -4185,7 +4185,7 @@
         <v>9</v>
       </c>
       <c r="G22" s="1" t="b">
-        <f>(B22=J22)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I22" s="1" t="s">
@@ -4221,7 +4221,7 @@
         <v>9</v>
       </c>
       <c r="G23" s="1" t="b">
-        <f>(B23=J23)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I23" s="1" t="s">
@@ -4257,7 +4257,7 @@
         <v>9</v>
       </c>
       <c r="G24" s="1" t="b">
-        <f>(B24=J24)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I24" s="1" t="s">
@@ -4293,7 +4293,7 @@
         <v>513</v>
       </c>
       <c r="G25" s="1" t="b">
-        <f>(B25=J25)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I25" s="1" t="s">
@@ -4329,7 +4329,7 @@
         <v>513</v>
       </c>
       <c r="G26" s="1" t="b">
-        <f>(B26=J26)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I26" s="1" t="s">
@@ -4365,7 +4365,7 @@
         <v>513</v>
       </c>
       <c r="G27" s="1" t="b">
-        <f>(B27=J27)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -4401,7 +4401,7 @@
         <v>513</v>
       </c>
       <c r="G28" s="1" t="b">
-        <f>(B28=J28)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -4437,7 +4437,7 @@
         <v>513</v>
       </c>
       <c r="G29" s="1" t="b">
-        <f>(B29=J29)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I29" s="1" t="s">
@@ -4473,7 +4473,7 @@
         <v>513</v>
       </c>
       <c r="G30" s="1" t="b">
-        <f>(B30=J30)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I30" s="1" t="s">
@@ -4509,7 +4509,7 @@
         <v>513</v>
       </c>
       <c r="G31" s="1" t="b">
-        <f>(B31=J31)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I31" s="1" t="s">
@@ -4545,7 +4545,7 @@
         <v>513</v>
       </c>
       <c r="G32" s="1" t="b">
-        <f>(B32=J32)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I32" s="1" t="s">
@@ -4581,7 +4581,7 @@
         <v>513</v>
       </c>
       <c r="G33" s="1" t="b">
-        <f>(B33=J33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I33" s="1" t="s">
@@ -4617,7 +4617,7 @@
         <v>513</v>
       </c>
       <c r="G34" s="1" t="b">
-        <f>(B34=J34)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I34" s="1" t="s">
@@ -4653,7 +4653,7 @@
         <v>513</v>
       </c>
       <c r="G35" s="1" t="b">
-        <f>(B35=J35)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I35" s="1" t="s">
@@ -4689,7 +4689,7 @@
         <v>513</v>
       </c>
       <c r="G36" s="1" t="b">
-        <f>(B36=J36)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -4725,7 +4725,7 @@
         <v>513</v>
       </c>
       <c r="G37" s="1" t="b">
-        <f>(B37=J37)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I37" s="1" t="s">
@@ -4761,7 +4761,7 @@
         <v>513</v>
       </c>
       <c r="G38" s="1" t="b">
-        <f>(B38=J38)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I38" s="1" t="s">
@@ -4797,7 +4797,7 @@
         <v>513</v>
       </c>
       <c r="G39" s="1" t="b">
-        <f>(B39=J39)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I39" s="1" t="s">
@@ -4833,7 +4833,7 @@
         <v>513</v>
       </c>
       <c r="G40" s="1" t="b">
-        <f>(B40=J40)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I40" s="1" t="s">
@@ -4869,7 +4869,7 @@
         <v>513</v>
       </c>
       <c r="G41" s="1" t="b">
-        <f>(B41=J41)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I41" s="1" t="s">
@@ -4905,7 +4905,7 @@
         <v>513</v>
       </c>
       <c r="G42" s="1" t="b">
-        <f>(B42=J42)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I42" s="1" t="s">
@@ -4941,7 +4941,7 @@
         <v>513</v>
       </c>
       <c r="G43" s="1" t="b">
-        <f>(B43=J43)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I43" s="1" t="s">
@@ -4977,7 +4977,7 @@
         <v>513</v>
       </c>
       <c r="G44" s="1" t="b">
-        <f>(B44=J44)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I44" s="1" t="s">
@@ -5013,7 +5013,7 @@
         <v>513</v>
       </c>
       <c r="G45" s="1" t="b">
-        <f>(B45=J45)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I45" s="1" t="s">
@@ -5049,7 +5049,7 @@
         <v>513</v>
       </c>
       <c r="G46" s="1" t="b">
-        <f>(B46=J46)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I46" s="1" t="s">
@@ -5085,7 +5085,7 @@
         <v>513</v>
       </c>
       <c r="G47" s="1" t="b">
-        <f>(B47=J47)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -5121,7 +5121,7 @@
         <v>513</v>
       </c>
       <c r="G48" s="1" t="b">
-        <f>(B48=J48)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I48" s="1" t="s">
@@ -5157,7 +5157,7 @@
         <v>513</v>
       </c>
       <c r="G49" s="1" t="b">
-        <f>(B49=J49)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I49" s="1" t="s">
@@ -5193,7 +5193,7 @@
         <v>513</v>
       </c>
       <c r="G50" s="1" t="b">
-        <f>(B50=J50)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I50" s="1" t="s">
@@ -5229,7 +5229,7 @@
         <v>513</v>
       </c>
       <c r="G51" s="1" t="b">
-        <f>(B51=J51)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I51" s="1" t="s">
@@ -5265,7 +5265,7 @@
         <v>513</v>
       </c>
       <c r="G52" s="1" t="b">
-        <f>(B52=J52)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I52" s="1" t="s">
@@ -5301,7 +5301,7 @@
         <v>513</v>
       </c>
       <c r="G53" s="1" t="b">
-        <f>(B53=J53)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I53" s="1" t="s">
@@ -5337,7 +5337,7 @@
         <v>513</v>
       </c>
       <c r="G54" s="1" t="b">
-        <f>(B54=J54)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I54" s="1" t="s">
@@ -5373,7 +5373,7 @@
         <v>513</v>
       </c>
       <c r="G55" s="1" t="b">
-        <f>(B55=J55)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I55" s="1" t="s">
@@ -5409,7 +5409,7 @@
         <v>513</v>
       </c>
       <c r="G56" s="1" t="b">
-        <f>(B56=J56)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I56" s="1" t="s">
@@ -5445,7 +5445,7 @@
         <v>513</v>
       </c>
       <c r="G57" s="1" t="b">
-        <f>(B57=J57)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I57" s="1" t="s">
@@ -5481,7 +5481,7 @@
         <v>513</v>
       </c>
       <c r="G58" s="1" t="b">
-        <f>(B58=J58)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I58" s="1" t="s">
@@ -5517,7 +5517,7 @@
         <v>513</v>
       </c>
       <c r="G59" s="1" t="b">
-        <f>(B59=J59)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I59" s="1" t="s">
@@ -5553,7 +5553,7 @@
         <v>513</v>
       </c>
       <c r="G60" s="1" t="b">
-        <f>(B60=J60)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I60" s="1" t="s">
@@ -5589,7 +5589,7 @@
         <v>513</v>
       </c>
       <c r="G61" s="1" t="b">
-        <f>(B61=J61)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I61" s="1" t="s">
@@ -5625,7 +5625,7 @@
         <v>513</v>
       </c>
       <c r="G62" s="1" t="b">
-        <f>(B62=J62)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I62" s="1" t="s">
@@ -5661,7 +5661,7 @@
         <v>513</v>
       </c>
       <c r="G63" s="1" t="b">
-        <f>(B63=J63)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I63" s="1" t="s">
@@ -5697,7 +5697,7 @@
         <v>513</v>
       </c>
       <c r="G64" s="1" t="b">
-        <f>(B64=J64)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I64" s="1" t="s">
@@ -5733,7 +5733,7 @@
         <v>513</v>
       </c>
       <c r="G65" s="1" t="b">
-        <f>(B65=J65)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I65" s="1" t="s">
@@ -5769,7 +5769,7 @@
         <v>513</v>
       </c>
       <c r="G66" s="1" t="b">
-        <f>(B66=J66)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I66" s="1" t="s">
@@ -5805,7 +5805,7 @@
         <v>513</v>
       </c>
       <c r="G67" s="1" t="b">
-        <f>(B67=J67)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I67" s="1" t="s">
@@ -5841,7 +5841,7 @@
         <v>513</v>
       </c>
       <c r="G68" s="1" t="b">
-        <f>(B68=J68)</f>
+        <f t="shared" ref="G68:G131" si="1">(B68=J68)</f>
         <v>1</v>
       </c>
       <c r="I68" s="1" t="s">
@@ -5877,7 +5877,7 @@
         <v>513</v>
       </c>
       <c r="G69" s="1" t="b">
-        <f>(B69=J69)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I69" s="1" t="s">
@@ -5913,7 +5913,7 @@
         <v>513</v>
       </c>
       <c r="G70" s="1" t="b">
-        <f>(B70=J70)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I70" s="1" t="s">
@@ -5949,7 +5949,7 @@
         <v>513</v>
       </c>
       <c r="G71" s="1" t="b">
-        <f>(B71=J71)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I71" s="1" t="s">
@@ -5985,7 +5985,7 @@
         <v>513</v>
       </c>
       <c r="G72" s="1" t="b">
-        <f>(B72=J72)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I72" s="1" t="s">
@@ -6021,7 +6021,7 @@
         <v>513</v>
       </c>
       <c r="G73" s="1" t="b">
-        <f>(B73=J73)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I73" s="1" t="s">
@@ -6057,7 +6057,7 @@
         <v>513</v>
       </c>
       <c r="G74" s="1" t="b">
-        <f>(B74=J74)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I74" s="1" t="s">
@@ -6093,7 +6093,7 @@
         <v>513</v>
       </c>
       <c r="G75" s="1" t="b">
-        <f>(B75=J75)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I75" s="1" t="s">
@@ -6129,7 +6129,7 @@
         <v>513</v>
       </c>
       <c r="G76" s="1" t="b">
-        <f>(B76=J76)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I76" s="1" t="s">
@@ -6165,7 +6165,7 @@
         <v>513</v>
       </c>
       <c r="G77" s="1" t="b">
-        <f>(B77=J77)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I77" s="1" t="s">
@@ -6201,7 +6201,7 @@
         <v>513</v>
       </c>
       <c r="G78" s="1" t="b">
-        <f>(B78=J78)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I78" s="1" t="s">
@@ -6237,7 +6237,7 @@
         <v>513</v>
       </c>
       <c r="G79" s="1" t="b">
-        <f>(B79=J79)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I79" s="1" t="s">
@@ -6273,7 +6273,7 @@
         <v>513</v>
       </c>
       <c r="G80" s="1" t="b">
-        <f>(B80=J80)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I80" s="1" t="s">
@@ -6309,7 +6309,7 @@
         <v>513</v>
       </c>
       <c r="G81" s="1" t="b">
-        <f>(B81=J81)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I81" s="1" t="s">
@@ -6345,7 +6345,7 @@
         <v>513</v>
       </c>
       <c r="G82" s="1" t="b">
-        <f>(B82=J82)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I82" s="1" t="s">
@@ -6381,7 +6381,7 @@
         <v>513</v>
       </c>
       <c r="G83" s="1" t="b">
-        <f>(B83=J83)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I83" s="1" t="s">
@@ -6417,7 +6417,7 @@
         <v>513</v>
       </c>
       <c r="G84" s="1" t="b">
-        <f>(B84=J84)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I84" s="1" t="s">
@@ -6453,7 +6453,7 @@
         <v>513</v>
       </c>
       <c r="G85" s="1" t="b">
-        <f>(B85=J85)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I85" s="1" t="s">
@@ -6489,7 +6489,7 @@
         <v>513</v>
       </c>
       <c r="G86" s="1" t="b">
-        <f>(B86=J86)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I86" s="1" t="s">
@@ -6525,7 +6525,7 @@
         <v>513</v>
       </c>
       <c r="G87" s="1" t="b">
-        <f>(B87=J87)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I87" s="1" t="s">
@@ -6561,7 +6561,7 @@
         <v>513</v>
       </c>
       <c r="G88" s="1" t="b">
-        <f>(B88=J88)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I88" s="1" t="s">
@@ -6597,7 +6597,7 @@
         <v>513</v>
       </c>
       <c r="G89" s="1" t="b">
-        <f>(B89=J89)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I89" s="1" t="s">
@@ -6633,7 +6633,7 @@
         <v>513</v>
       </c>
       <c r="G90" s="1" t="b">
-        <f>(B90=J90)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I90" s="1" t="s">
@@ -6669,7 +6669,7 @@
         <v>513</v>
       </c>
       <c r="G91" s="1" t="b">
-        <f>(B91=J91)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I91" s="1" t="s">
@@ -6705,7 +6705,7 @@
         <v>513</v>
       </c>
       <c r="G92" s="1" t="b">
-        <f>(B92=J92)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I92" s="1" t="s">
@@ -6741,7 +6741,7 @@
         <v>513</v>
       </c>
       <c r="G93" s="1" t="b">
-        <f>(B93=J93)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I93" s="1" t="s">
@@ -6777,7 +6777,7 @@
         <v>513</v>
       </c>
       <c r="G94" s="1" t="b">
-        <f>(B94=J94)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I94" s="1" t="s">
@@ -6813,7 +6813,7 @@
         <v>513</v>
       </c>
       <c r="G95" s="1" t="b">
-        <f>(B95=J95)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I95" s="1" t="s">
@@ -6849,7 +6849,7 @@
         <v>513</v>
       </c>
       <c r="G96" s="1" t="b">
-        <f>(B96=J96)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I96" s="1" t="s">
@@ -6885,7 +6885,7 @@
         <v>513</v>
       </c>
       <c r="G97" s="1" t="b">
-        <f>(B97=J97)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I97" s="1" t="s">
@@ -6921,7 +6921,7 @@
         <v>513</v>
       </c>
       <c r="G98" s="1" t="b">
-        <f>(B98=J98)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I98" s="1" t="s">
@@ -6957,7 +6957,7 @@
         <v>513</v>
       </c>
       <c r="G99" s="1" t="b">
-        <f>(B99=J99)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I99" s="1" t="s">
@@ -6994,7 +6994,7 @@
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2" t="b">
-        <f>(B100=J100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H100" s="2"/>
@@ -7031,7 +7031,7 @@
         <v>353</v>
       </c>
       <c r="G101" s="1" t="b">
-        <f>(B101=J101)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I101" s="1" t="s">
@@ -7067,7 +7067,7 @@
         <v>353</v>
       </c>
       <c r="G102" s="1" t="b">
-        <f>(B102=J102)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I102" s="1" t="s">
@@ -7103,7 +7103,7 @@
         <v>353</v>
       </c>
       <c r="G103" s="1" t="b">
-        <f>(B103=J103)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I103" s="1" t="s">
@@ -7139,7 +7139,7 @@
         <v>353</v>
       </c>
       <c r="G104" s="1" t="b">
-        <f>(B104=J104)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I104" s="1" t="s">
@@ -7175,7 +7175,7 @@
         <v>353</v>
       </c>
       <c r="G105" s="1" t="b">
-        <f>(B105=J105)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I105" s="1" t="s">
@@ -7211,7 +7211,7 @@
         <v>353</v>
       </c>
       <c r="G106" s="1" t="b">
-        <f>(B106=J106)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I106" s="1" t="s">
@@ -7247,7 +7247,7 @@
         <v>353</v>
       </c>
       <c r="G107" s="1" t="b">
-        <f>(B107=J107)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I107" s="1" t="s">
@@ -7283,7 +7283,7 @@
         <v>353</v>
       </c>
       <c r="G108" s="1" t="b">
-        <f>(B108=J108)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I108" s="1" t="s">
@@ -7319,7 +7319,7 @@
         <v>353</v>
       </c>
       <c r="G109" s="1" t="b">
-        <f>(B109=J109)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I109" s="1" t="s">
@@ -7355,7 +7355,7 @@
         <v>353</v>
       </c>
       <c r="G110" s="1" t="b">
-        <f>(B110=J110)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I110" s="1" t="s">
@@ -7391,7 +7391,7 @@
         <v>353</v>
       </c>
       <c r="G111" s="1" t="b">
-        <f>(B111=J111)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I111" s="1" t="s">
@@ -7427,7 +7427,7 @@
         <v>353</v>
       </c>
       <c r="G112" s="1" t="b">
-        <f>(B112=J112)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I112" s="1" t="s">
@@ -7463,7 +7463,7 @@
         <v>353</v>
       </c>
       <c r="G113" s="1" t="b">
-        <f>(B113=J113)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I113" s="1" t="s">
@@ -7499,7 +7499,7 @@
         <v>353</v>
       </c>
       <c r="G114" s="1" t="b">
-        <f>(B114=J114)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I114" s="1" t="s">
@@ -7535,7 +7535,7 @@
         <v>353</v>
       </c>
       <c r="G115" s="1" t="b">
-        <f>(B115=J115)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I115" s="1" t="s">
@@ -7571,7 +7571,7 @@
         <v>353</v>
       </c>
       <c r="G116" s="1" t="b">
-        <f>(B116=J116)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I116" s="1" t="s">
@@ -7607,7 +7607,7 @@
         <v>353</v>
       </c>
       <c r="G117" s="1" t="b">
-        <f>(B117=J117)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I117" s="1" t="s">
@@ -7643,7 +7643,7 @@
         <v>353</v>
       </c>
       <c r="G118" s="1" t="b">
-        <f>(B118=J118)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I118" s="1" t="s">
@@ -7679,7 +7679,7 @@
         <v>353</v>
       </c>
       <c r="G119" s="1" t="b">
-        <f>(B119=J119)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I119" s="1" t="s">
@@ -7715,7 +7715,7 @@
         <v>353</v>
       </c>
       <c r="G120" s="1" t="b">
-        <f>(B120=J120)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I120" s="1" t="s">
@@ -7751,7 +7751,7 @@
         <v>353</v>
       </c>
       <c r="G121" s="1" t="b">
-        <f>(B121=J121)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I121" s="1" t="s">
@@ -7787,7 +7787,7 @@
         <v>52</v>
       </c>
       <c r="G122" s="1" t="b">
-        <f>(B122=J122)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I122" s="1" t="s">
@@ -7823,7 +7823,7 @@
         <v>52</v>
       </c>
       <c r="G123" s="1" t="b">
-        <f>(B123=J123)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I123" s="1" t="s">
@@ -7859,7 +7859,7 @@
         <v>52</v>
       </c>
       <c r="G124" s="1" t="b">
-        <f>(B124=J124)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I124" s="1" t="s">
@@ -7895,7 +7895,7 @@
         <v>52</v>
       </c>
       <c r="G125" s="1" t="b">
-        <f>(B125=J125)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I125" s="1" t="s">
@@ -7931,7 +7931,7 @@
         <v>52</v>
       </c>
       <c r="G126" s="1" t="b">
-        <f>(B126=J126)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I126" s="1" t="s">
@@ -7967,7 +7967,7 @@
         <v>52</v>
       </c>
       <c r="G127" s="1" t="b">
-        <f>(B127=J127)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I127" s="1" t="s">
@@ -8003,7 +8003,7 @@
         <v>52</v>
       </c>
       <c r="G128" s="1" t="b">
-        <f>(B128=J128)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I128" s="1" t="s">
@@ -8039,7 +8039,7 @@
         <v>52</v>
       </c>
       <c r="G129" s="1" t="b">
-        <f>(B129=J129)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I129" s="1" t="s">
@@ -8075,7 +8075,7 @@
         <v>52</v>
       </c>
       <c r="G130" s="1" t="b">
-        <f>(B130=J130)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I130" s="1" t="s">
@@ -8111,7 +8111,7 @@
         <v>52</v>
       </c>
       <c r="G131" s="1" t="b">
-        <f>(B131=J131)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I131" s="1" t="s">
@@ -8147,7 +8147,7 @@
         <v>52</v>
       </c>
       <c r="G132" s="1" t="b">
-        <f>(B132=J132)</f>
+        <f t="shared" ref="G132:G195" si="2">(B132=J132)</f>
         <v>1</v>
       </c>
       <c r="I132" s="1" t="s">
@@ -8183,7 +8183,7 @@
         <v>52</v>
       </c>
       <c r="G133" s="1" t="b">
-        <f>(B133=J133)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I133" s="1" t="s">
@@ -8219,7 +8219,7 @@
         <v>52</v>
       </c>
       <c r="G134" s="1" t="b">
-        <f>(B134=J134)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I134" s="1" t="s">
@@ -8255,7 +8255,7 @@
         <v>52</v>
       </c>
       <c r="G135" s="1" t="b">
-        <f>(B135=J135)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I135" s="1" t="s">
@@ -8291,7 +8291,7 @@
         <v>52</v>
       </c>
       <c r="G136" s="1" t="b">
-        <f>(B136=J136)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I136" s="1" t="s">
@@ -8327,7 +8327,7 @@
         <v>52</v>
       </c>
       <c r="G137" s="1" t="b">
-        <f>(B137=J137)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I137" s="1" t="s">
@@ -8363,7 +8363,7 @@
         <v>52</v>
       </c>
       <c r="G138" s="1" t="b">
-        <f>(B138=J138)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I138" s="1" t="s">
@@ -8399,7 +8399,7 @@
         <v>52</v>
       </c>
       <c r="G139" s="1" t="b">
-        <f>(B139=J139)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I139" s="1" t="s">
@@ -8435,7 +8435,7 @@
         <v>52</v>
       </c>
       <c r="G140" s="1" t="b">
-        <f>(B140=J140)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I140" s="1" t="s">
@@ -8471,7 +8471,7 @@
         <v>52</v>
       </c>
       <c r="G141" s="1" t="b">
-        <f>(B141=J141)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I141" s="1" t="s">
@@ -8507,7 +8507,7 @@
         <v>52</v>
       </c>
       <c r="G142" s="1" t="b">
-        <f>(B142=J142)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I142" s="1" t="s">
@@ -8543,7 +8543,7 @@
         <v>52</v>
       </c>
       <c r="G143" s="1" t="b">
-        <f>(B143=J143)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I143" s="1" t="s">
@@ -8579,7 +8579,7 @@
         <v>52</v>
       </c>
       <c r="G144" s="1" t="b">
-        <f>(B144=J144)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I144" s="1" t="s">
@@ -8615,7 +8615,7 @@
         <v>52</v>
       </c>
       <c r="G145" s="1" t="b">
-        <f>(B145=J145)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I145" s="1" t="s">
@@ -8651,7 +8651,7 @@
         <v>52</v>
       </c>
       <c r="G146" s="1" t="b">
-        <f>(B146=J146)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I146" s="1" t="s">
@@ -8687,7 +8687,7 @@
         <v>52</v>
       </c>
       <c r="G147" s="1" t="b">
-        <f>(B147=J147)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I147" s="1" t="s">
@@ -8723,7 +8723,7 @@
         <v>52</v>
       </c>
       <c r="G148" s="1" t="b">
-        <f>(B148=J148)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I148" s="1" t="s">
@@ -8759,7 +8759,7 @@
         <v>52</v>
       </c>
       <c r="G149" s="1" t="b">
-        <f>(B149=J149)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I149" s="1" t="s">
@@ -8795,7 +8795,7 @@
         <v>52</v>
       </c>
       <c r="G150" s="1" t="b">
-        <f>(B150=J150)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I150" s="1" t="s">
@@ -8831,7 +8831,7 @@
         <v>52</v>
       </c>
       <c r="G151" s="1" t="b">
-        <f>(B151=J151)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I151" s="1" t="s">
@@ -8867,7 +8867,7 @@
         <v>52</v>
       </c>
       <c r="G152" s="1" t="b">
-        <f>(B152=J152)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I152" s="1" t="s">
@@ -8903,7 +8903,7 @@
         <v>52</v>
       </c>
       <c r="G153" s="1" t="b">
-        <f>(B153=J153)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I153" s="1" t="s">
@@ -8939,7 +8939,7 @@
         <v>52</v>
       </c>
       <c r="G154" s="1" t="b">
-        <f>(B154=J154)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I154" s="1" t="s">
@@ -8975,7 +8975,7 @@
         <v>52</v>
       </c>
       <c r="G155" s="1" t="b">
-        <f>(B155=J155)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I155" s="1" t="s">
@@ -9011,7 +9011,7 @@
         <v>52</v>
       </c>
       <c r="G156" s="1" t="b">
-        <f>(B156=J156)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I156" s="1" t="s">
@@ -9047,7 +9047,7 @@
         <v>52</v>
       </c>
       <c r="G157" s="1" t="b">
-        <f>(B157=J157)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I157" s="1" t="s">
@@ -9083,7 +9083,7 @@
         <v>52</v>
       </c>
       <c r="G158" s="1" t="b">
-        <f>(B158=J158)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I158" s="1" t="s">
@@ -9119,7 +9119,7 @@
         <v>52</v>
       </c>
       <c r="G159" s="1" t="b">
-        <f>(B159=J159)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I159" s="1" t="s">
@@ -9155,7 +9155,7 @@
         <v>52</v>
       </c>
       <c r="G160" s="1" t="b">
-        <f>(B160=J160)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I160" s="1" t="s">
@@ -9191,7 +9191,7 @@
         <v>52</v>
       </c>
       <c r="G161" s="1" t="b">
-        <f>(B161=J161)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I161" s="1" t="s">
@@ -9227,7 +9227,7 @@
         <v>52</v>
       </c>
       <c r="G162" s="1" t="b">
-        <f>(B162=J162)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I162" s="1" t="s">
@@ -9263,7 +9263,7 @@
         <v>52</v>
       </c>
       <c r="G163" s="1" t="b">
-        <f>(B163=J163)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I163" s="1" t="s">
@@ -9299,7 +9299,7 @@
         <v>52</v>
       </c>
       <c r="G164" s="1" t="b">
-        <f>(B164=J164)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I164" s="1" t="s">
@@ -9335,7 +9335,7 @@
         <v>52</v>
       </c>
       <c r="G165" s="1" t="b">
-        <f>(B165=J165)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I165" s="1" t="s">
@@ -9371,7 +9371,7 @@
         <v>52</v>
       </c>
       <c r="G166" s="1" t="b">
-        <f>(B166=J166)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I166" s="1" t="s">
@@ -9407,7 +9407,7 @@
         <v>52</v>
       </c>
       <c r="G167" s="1" t="b">
-        <f>(B167=J167)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I167" s="1" t="s">
@@ -9443,7 +9443,7 @@
         <v>52</v>
       </c>
       <c r="G168" s="1" t="b">
-        <f>(B168=J168)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I168" s="1" t="s">
@@ -9479,7 +9479,7 @@
         <v>52</v>
       </c>
       <c r="G169" s="1" t="b">
-        <f>(B169=J169)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I169" s="1" t="s">
@@ -9515,7 +9515,7 @@
         <v>52</v>
       </c>
       <c r="G170" s="1" t="b">
-        <f>(B170=J170)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I170" s="1" t="s">
@@ -9551,7 +9551,7 @@
         <v>52</v>
       </c>
       <c r="G171" s="1" t="b">
-        <f>(B171=J171)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I171" s="1" t="s">
@@ -9587,7 +9587,7 @@
         <v>52</v>
       </c>
       <c r="G172" s="1" t="b">
-        <f>(B172=J172)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I172" s="1" t="s">
@@ -9623,7 +9623,7 @@
         <v>52</v>
       </c>
       <c r="G173" s="1" t="b">
-        <f>(B173=J173)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I173" s="1" t="s">
@@ -9659,7 +9659,7 @@
         <v>52</v>
       </c>
       <c r="G174" s="1" t="b">
-        <f>(B174=J174)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I174" s="1" t="s">
@@ -9695,7 +9695,7 @@
         <v>52</v>
       </c>
       <c r="G175" s="1" t="b">
-        <f>(B175=J175)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I175" s="1" t="s">
@@ -9731,7 +9731,7 @@
         <v>52</v>
       </c>
       <c r="G176" s="1" t="b">
-        <f>(B176=J176)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I176" s="1" t="s">
@@ -9767,7 +9767,7 @@
         <v>52</v>
       </c>
       <c r="G177" s="1" t="b">
-        <f>(B177=J177)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I177" s="1" t="s">
@@ -9803,7 +9803,7 @@
         <v>52</v>
       </c>
       <c r="G178" s="1" t="b">
-        <f>(B178=J178)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I178" s="1" t="s">
@@ -9839,7 +9839,7 @@
         <v>52</v>
       </c>
       <c r="G179" s="1" t="b">
-        <f>(B179=J179)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I179" s="1" t="s">
@@ -9875,7 +9875,7 @@
         <v>52</v>
       </c>
       <c r="G180" s="1" t="b">
-        <f>(B180=J180)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I180" s="1" t="s">
@@ -9911,7 +9911,7 @@
         <v>52</v>
       </c>
       <c r="G181" s="1" t="b">
-        <f>(B181=J181)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I181" s="1" t="s">
@@ -9947,7 +9947,7 @@
         <v>52</v>
       </c>
       <c r="G182" s="1" t="b">
-        <f>(B182=J182)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I182" s="1" t="s">
@@ -9983,7 +9983,7 @@
         <v>52</v>
       </c>
       <c r="G183" s="1" t="b">
-        <f>(B183=J183)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I183" s="1" t="s">
@@ -10019,7 +10019,7 @@
         <v>52</v>
       </c>
       <c r="G184" s="1" t="b">
-        <f>(B184=J184)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I184" s="1" t="s">
@@ -10055,7 +10055,7 @@
         <v>52</v>
       </c>
       <c r="G185" s="1" t="b">
-        <f>(B185=J185)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I185" s="1" t="s">
@@ -10091,7 +10091,7 @@
         <v>52</v>
       </c>
       <c r="G186" s="1" t="b">
-        <f>(B186=J186)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I186" s="1" t="s">
@@ -10127,7 +10127,7 @@
         <v>52</v>
       </c>
       <c r="G187" s="1" t="b">
-        <f>(B187=J187)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I187" s="1" t="s">
@@ -10163,7 +10163,7 @@
         <v>52</v>
       </c>
       <c r="G188" s="1" t="b">
-        <f>(B188=J188)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I188" s="1" t="s">
@@ -10199,7 +10199,7 @@
         <v>52</v>
       </c>
       <c r="G189" s="1" t="b">
-        <f>(B189=J189)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I189" s="1" t="s">
@@ -10235,7 +10235,7 @@
         <v>52</v>
       </c>
       <c r="G190" s="1" t="b">
-        <f>(B190=J190)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I190" s="1" t="s">
@@ -10271,7 +10271,7 @@
         <v>52</v>
       </c>
       <c r="G191" s="1" t="b">
-        <f>(B191=J191)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I191" s="1" t="s">
@@ -10307,7 +10307,7 @@
         <v>52</v>
       </c>
       <c r="G192" s="1" t="b">
-        <f>(B192=J192)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I192" s="1" t="s">
@@ -10343,7 +10343,7 @@
         <v>52</v>
       </c>
       <c r="G193" s="1" t="b">
-        <f>(B193=J193)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I193" s="1" t="s">
@@ -10379,7 +10379,7 @@
         <v>52</v>
       </c>
       <c r="G194" s="1" t="b">
-        <f>(B194=J194)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I194" s="1" t="s">
@@ -10415,7 +10415,7 @@
         <v>52</v>
       </c>
       <c r="G195" s="1" t="b">
-        <f>(B195=J195)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I195" s="1" t="s">
@@ -10451,7 +10451,7 @@
         <v>52</v>
       </c>
       <c r="G196" s="1" t="b">
-        <f>(B196=J196)</f>
+        <f t="shared" ref="G196:G259" si="3">(B196=J196)</f>
         <v>1</v>
       </c>
       <c r="I196" s="1" t="s">
@@ -10487,7 +10487,7 @@
         <v>52</v>
       </c>
       <c r="G197" s="1" t="b">
-        <f>(B197=J197)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I197" s="1" t="s">
@@ -10523,7 +10523,7 @@
         <v>52</v>
       </c>
       <c r="G198" s="1" t="b">
-        <f>(B198=J198)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I198" s="1" t="s">
@@ -10559,7 +10559,7 @@
         <v>52</v>
       </c>
       <c r="G199" s="1" t="b">
-        <f>(B199=J199)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I199" s="1" t="s">
@@ -10595,7 +10595,7 @@
         <v>52</v>
       </c>
       <c r="G200" s="1" t="b">
-        <f>(B200=J200)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I200" s="1" t="s">
@@ -10631,7 +10631,7 @@
         <v>52</v>
       </c>
       <c r="G201" s="1" t="b">
-        <f>(B201=J201)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I201" s="1" t="s">
@@ -10667,7 +10667,7 @@
         <v>52</v>
       </c>
       <c r="G202" s="1" t="b">
-        <f>(B202=J202)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I202" s="1" t="s">
@@ -10703,7 +10703,7 @@
         <v>52</v>
       </c>
       <c r="G203" s="1" t="b">
-        <f>(B203=J203)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I203" s="1" t="s">
@@ -10739,7 +10739,7 @@
         <v>52</v>
       </c>
       <c r="G204" s="1" t="b">
-        <f>(B204=J204)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I204" s="1" t="s">
@@ -10775,7 +10775,7 @@
         <v>52</v>
       </c>
       <c r="G205" s="1" t="b">
-        <f>(B205=J205)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I205" s="1" t="s">
@@ -10811,7 +10811,7 @@
         <v>52</v>
       </c>
       <c r="G206" s="1" t="b">
-        <f>(B206=J206)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I206" s="1" t="s">
@@ -10847,7 +10847,7 @@
         <v>52</v>
       </c>
       <c r="G207" s="1" t="b">
-        <f>(B207=J207)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I207" s="1" t="s">
@@ -10883,7 +10883,7 @@
         <v>52</v>
       </c>
       <c r="G208" s="1" t="b">
-        <f>(B208=J208)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I208" s="1" t="s">
@@ -10919,7 +10919,7 @@
         <v>52</v>
       </c>
       <c r="G209" s="1" t="b">
-        <f>(B209=J209)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I209" s="1" t="s">
@@ -10955,7 +10955,7 @@
         <v>52</v>
       </c>
       <c r="G210" s="1" t="b">
-        <f>(B210=J210)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I210" s="1" t="s">
@@ -10991,7 +10991,7 @@
         <v>52</v>
       </c>
       <c r="G211" s="1" t="b">
-        <f>(B211=J211)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I211" s="1" t="s">
@@ -11027,7 +11027,7 @@
         <v>52</v>
       </c>
       <c r="G212" s="1" t="b">
-        <f>(B212=J212)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I212" s="1" t="s">
@@ -11063,7 +11063,7 @@
         <v>52</v>
       </c>
       <c r="G213" s="1" t="b">
-        <f>(B213=J213)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I213" s="1" t="s">
@@ -11099,7 +11099,7 @@
         <v>52</v>
       </c>
       <c r="G214" s="1" t="b">
-        <f>(B214=J214)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I214" s="1" t="s">
@@ -11135,7 +11135,7 @@
         <v>52</v>
       </c>
       <c r="G215" s="1" t="b">
-        <f>(B215=J215)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I215" s="1" t="s">
@@ -11171,7 +11171,7 @@
         <v>52</v>
       </c>
       <c r="G216" s="1" t="b">
-        <f>(B216=J216)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I216" s="1" t="s">
@@ -11207,7 +11207,7 @@
         <v>52</v>
       </c>
       <c r="G217" s="1" t="b">
-        <f>(B217=J217)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I217" s="1" t="s">
@@ -11243,7 +11243,7 @@
         <v>52</v>
       </c>
       <c r="G218" s="1" t="b">
-        <f>(B218=J218)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I218" s="1" t="s">
@@ -11279,7 +11279,7 @@
         <v>52</v>
       </c>
       <c r="G219" s="1" t="b">
-        <f>(B219=J219)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I219" s="1" t="s">
@@ -11315,7 +11315,7 @@
         <v>52</v>
       </c>
       <c r="G220" s="1" t="b">
-        <f>(B220=J220)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I220" s="1" t="s">
@@ -11351,7 +11351,7 @@
         <v>52</v>
       </c>
       <c r="G221" s="1" t="b">
-        <f>(B221=J221)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I221" s="1" t="s">
@@ -11387,7 +11387,7 @@
         <v>52</v>
       </c>
       <c r="G222" s="1" t="b">
-        <f>(B222=J222)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I222" s="1" t="s">
@@ -11423,7 +11423,7 @@
         <v>52</v>
       </c>
       <c r="G223" s="1" t="b">
-        <f>(B223=J223)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I223" s="1" t="s">
@@ -11459,7 +11459,7 @@
         <v>52</v>
       </c>
       <c r="G224" s="1" t="b">
-        <f>(B224=J224)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I224" s="1" t="s">
@@ -11495,7 +11495,7 @@
         <v>52</v>
       </c>
       <c r="G225" s="1" t="b">
-        <f>(B225=J225)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I225" s="1" t="s">
@@ -11531,7 +11531,7 @@
         <v>52</v>
       </c>
       <c r="G226" s="1" t="b">
-        <f>(B226=J226)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I226" s="1" t="s">
@@ -11567,7 +11567,7 @@
         <v>52</v>
       </c>
       <c r="G227" s="1" t="b">
-        <f>(B227=J227)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I227" s="1" t="s">
@@ -11603,7 +11603,7 @@
         <v>52</v>
       </c>
       <c r="G228" s="1" t="b">
-        <f>(B228=J228)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I228" s="1" t="s">
@@ -11639,7 +11639,7 @@
         <v>52</v>
       </c>
       <c r="G229" s="1" t="b">
-        <f>(B229=J229)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I229" s="1" t="s">
@@ -11675,7 +11675,7 @@
         <v>52</v>
       </c>
       <c r="G230" s="1" t="b">
-        <f>(B230=J230)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I230" s="1" t="s">
@@ -11711,7 +11711,7 @@
         <v>52</v>
       </c>
       <c r="G231" s="1" t="b">
-        <f>(B231=J231)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I231" s="1" t="s">
@@ -11747,7 +11747,7 @@
         <v>52</v>
       </c>
       <c r="G232" s="1" t="b">
-        <f>(B232=J232)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I232" s="1" t="s">
@@ -11783,7 +11783,7 @@
         <v>52</v>
       </c>
       <c r="G233" s="1" t="b">
-        <f>(B233=J233)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I233" s="1" t="s">
@@ -11819,7 +11819,7 @@
         <v>52</v>
       </c>
       <c r="G234" s="1" t="b">
-        <f>(B234=J234)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I234" s="1" t="s">
@@ -11855,7 +11855,7 @@
         <v>52</v>
       </c>
       <c r="G235" s="1" t="b">
-        <f>(B235=J235)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I235" s="1" t="s">
@@ -11891,7 +11891,7 @@
         <v>52</v>
       </c>
       <c r="G236" s="1" t="b">
-        <f>(B236=J236)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I236" s="1" t="s">
@@ -11927,7 +11927,7 @@
         <v>52</v>
       </c>
       <c r="G237" s="1" t="b">
-        <f>(B237=J237)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I237" s="1" t="s">
@@ -11963,7 +11963,7 @@
         <v>52</v>
       </c>
       <c r="G238" s="1" t="b">
-        <f>(B238=J238)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I238" s="1" t="s">
@@ -11999,7 +11999,7 @@
         <v>52</v>
       </c>
       <c r="G239" s="1" t="b">
-        <f>(B239=J239)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I239" s="1" t="s">
@@ -12035,7 +12035,7 @@
         <v>52</v>
       </c>
       <c r="G240" s="1" t="b">
-        <f>(B240=J240)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I240" s="1" t="s">
@@ -12071,7 +12071,7 @@
         <v>52</v>
       </c>
       <c r="G241" s="1" t="b">
-        <f>(B241=J241)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I241" s="1" t="s">
@@ -12107,7 +12107,7 @@
         <v>52</v>
       </c>
       <c r="G242" s="1" t="b">
-        <f>(B242=J242)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I242" s="1" t="s">
@@ -12143,7 +12143,7 @@
         <v>52</v>
       </c>
       <c r="G243" s="1" t="b">
-        <f>(B243=J243)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I243" s="1" t="s">
@@ -12179,7 +12179,7 @@
         <v>52</v>
       </c>
       <c r="G244" s="1" t="b">
-        <f>(B244=J244)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I244" s="1" t="s">
@@ -12215,7 +12215,7 @@
         <v>52</v>
       </c>
       <c r="G245" s="1" t="b">
-        <f>(B245=J245)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I245" s="1" t="s">
@@ -12251,7 +12251,7 @@
         <v>52</v>
       </c>
       <c r="G246" s="1" t="b">
-        <f>(B246=J246)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I246" s="1" t="s">
@@ -12287,7 +12287,7 @@
         <v>52</v>
       </c>
       <c r="G247" s="1" t="b">
-        <f>(B247=J247)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I247" s="1" t="s">
@@ -12323,7 +12323,7 @@
         <v>52</v>
       </c>
       <c r="G248" s="1" t="b">
-        <f>(B248=J248)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I248" s="1" t="s">
@@ -12359,7 +12359,7 @@
         <v>52</v>
       </c>
       <c r="G249" s="1" t="b">
-        <f>(B249=J249)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I249" s="1" t="s">
@@ -12395,7 +12395,7 @@
         <v>52</v>
       </c>
       <c r="G250" s="1" t="b">
-        <f>(B250=J250)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I250" s="1" t="s">
@@ -12431,7 +12431,7 @@
         <v>52</v>
       </c>
       <c r="G251" s="1" t="b">
-        <f>(B251=J251)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I251" s="1" t="s">
@@ -12467,7 +12467,7 @@
         <v>52</v>
       </c>
       <c r="G252" s="1" t="b">
-        <f>(B252=J252)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I252" s="1" t="s">
@@ -12503,7 +12503,7 @@
         <v>52</v>
       </c>
       <c r="G253" s="1" t="b">
-        <f>(B253=J253)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I253" s="1" t="s">
@@ -12539,7 +12539,7 @@
         <v>52</v>
       </c>
       <c r="G254" s="1" t="b">
-        <f>(B254=J254)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I254" s="1" t="s">
@@ -12575,7 +12575,7 @@
         <v>52</v>
       </c>
       <c r="G255" s="1" t="b">
-        <f>(B255=J255)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I255" s="1" t="s">
@@ -12611,7 +12611,7 @@
         <v>52</v>
       </c>
       <c r="G256" s="1" t="b">
-        <f>(B256=J256)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I256" s="1" t="s">
@@ -12647,7 +12647,7 @@
         <v>52</v>
       </c>
       <c r="G257" s="1" t="b">
-        <f>(B257=J257)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I257" s="1" t="s">
@@ -12683,7 +12683,7 @@
         <v>52</v>
       </c>
       <c r="G258" s="1" t="b">
-        <f>(B258=J258)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I258" s="1" t="s">
@@ -12719,7 +12719,7 @@
         <v>52</v>
       </c>
       <c r="G259" s="1" t="b">
-        <f>(B259=J259)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I259" s="1" t="s">
@@ -12755,7 +12755,7 @@
         <v>52</v>
       </c>
       <c r="G260" s="1" t="b">
-        <f>(B260=J260)</f>
+        <f t="shared" ref="G260:G323" si="4">(B260=J260)</f>
         <v>1</v>
       </c>
       <c r="I260" s="1" t="s">
@@ -12791,7 +12791,7 @@
         <v>52</v>
       </c>
       <c r="G261" s="1" t="b">
-        <f>(B261=J261)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I261" s="1" t="s">
@@ -12827,7 +12827,7 @@
         <v>52</v>
       </c>
       <c r="G262" s="1" t="b">
-        <f>(B262=J262)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I262" s="1" t="s">
@@ -12863,7 +12863,7 @@
         <v>52</v>
       </c>
       <c r="G263" s="1" t="b">
-        <f>(B263=J263)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I263" s="1" t="s">
@@ -12899,7 +12899,7 @@
         <v>52</v>
       </c>
       <c r="G264" s="1" t="b">
-        <f>(B264=J264)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I264" s="1" t="s">
@@ -12935,7 +12935,7 @@
         <v>52</v>
       </c>
       <c r="G265" s="1" t="b">
-        <f>(B265=J265)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I265" s="1" t="s">
@@ -12971,7 +12971,7 @@
         <v>52</v>
       </c>
       <c r="G266" s="1" t="b">
-        <f>(B266=J266)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I266" s="1" t="s">
@@ -13007,7 +13007,7 @@
         <v>52</v>
       </c>
       <c r="G267" s="1" t="b">
-        <f>(B267=J267)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I267" s="1" t="s">
@@ -13043,7 +13043,7 @@
         <v>52</v>
       </c>
       <c r="G268" s="1" t="b">
-        <f>(B268=J268)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I268" s="1" t="s">
@@ -13079,7 +13079,7 @@
         <v>52</v>
       </c>
       <c r="G269" s="1" t="b">
-        <f>(B269=J269)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I269" s="1" t="s">
@@ -13115,7 +13115,7 @@
         <v>52</v>
       </c>
       <c r="G270" s="1" t="b">
-        <f>(B270=J270)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I270" s="1" t="s">
@@ -13151,7 +13151,7 @@
         <v>52</v>
       </c>
       <c r="G271" s="1" t="b">
-        <f>(B271=J271)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I271" s="1" t="s">
@@ -13187,7 +13187,7 @@
         <v>396</v>
       </c>
       <c r="G272" s="1" t="b">
-        <f>(B272=J272)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I272" s="1" t="s">
@@ -13223,7 +13223,7 @@
         <v>396</v>
       </c>
       <c r="G273" s="1" t="b">
-        <f>(B273=J273)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I273" s="1" t="s">
@@ -13259,7 +13259,7 @@
         <v>396</v>
       </c>
       <c r="G274" s="1" t="b">
-        <f>(B274=J274)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I274" s="1" t="s">
@@ -13295,7 +13295,7 @@
         <v>396</v>
       </c>
       <c r="G275" s="1" t="b">
-        <f>(B275=J275)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I275" s="1" t="s">
@@ -13331,7 +13331,7 @@
         <v>396</v>
       </c>
       <c r="G276" s="1" t="b">
-        <f>(B276=J276)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I276" s="1" t="s">
@@ -13367,7 +13367,7 @@
         <v>396</v>
       </c>
       <c r="G277" s="1" t="b">
-        <f>(B277=J277)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I277" s="1" t="s">
@@ -13403,7 +13403,7 @@
         <v>396</v>
       </c>
       <c r="G278" s="1" t="b">
-        <f>(B278=J278)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I278" s="1" t="s">
@@ -13439,7 +13439,7 @@
         <v>396</v>
       </c>
       <c r="G279" s="1" t="b">
-        <f>(B279=J279)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I279" s="1" t="s">
@@ -13475,7 +13475,7 @@
         <v>396</v>
       </c>
       <c r="G280" s="1" t="b">
-        <f>(B280=J280)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I280" s="1" t="s">
@@ -13511,7 +13511,7 @@
         <v>396</v>
       </c>
       <c r="G281" s="1" t="b">
-        <f>(B281=J281)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I281" s="1" t="s">
@@ -13547,7 +13547,7 @@
         <v>396</v>
       </c>
       <c r="G282" s="1" t="b">
-        <f>(B282=J282)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I282" s="1" t="s">
@@ -13583,7 +13583,7 @@
         <v>396</v>
       </c>
       <c r="G283" s="1" t="b">
-        <f>(B283=J283)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I283" s="1" t="s">
@@ -13619,7 +13619,7 @@
         <v>396</v>
       </c>
       <c r="G284" s="1" t="b">
-        <f>(B284=J284)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I284" s="1" t="s">
@@ -13655,7 +13655,7 @@
         <v>396</v>
       </c>
       <c r="G285" s="1" t="b">
-        <f>(B285=J285)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I285" s="1" t="s">
@@ -13691,7 +13691,7 @@
         <v>396</v>
       </c>
       <c r="G286" s="1" t="b">
-        <f>(B286=J286)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I286" s="1" t="s">
@@ -13727,7 +13727,7 @@
         <v>396</v>
       </c>
       <c r="G287" s="1" t="b">
-        <f>(B287=J287)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I287" s="1" t="s">
@@ -13763,7 +13763,7 @@
         <v>396</v>
       </c>
       <c r="G288" s="1" t="b">
-        <f>(B288=J288)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I288" s="1" t="s">
@@ -13799,7 +13799,7 @@
         <v>396</v>
       </c>
       <c r="G289" s="1" t="b">
-        <f>(B289=J289)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I289" s="1" t="s">
@@ -13835,7 +13835,7 @@
         <v>396</v>
       </c>
       <c r="G290" s="1" t="b">
-        <f>(B290=J290)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I290" s="1" t="s">
@@ -13871,7 +13871,7 @@
         <v>396</v>
       </c>
       <c r="G291" s="1" t="b">
-        <f>(B291=J291)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I291" s="1" t="s">
@@ -13907,7 +13907,7 @@
         <v>396</v>
       </c>
       <c r="G292" s="1" t="b">
-        <f>(B292=J292)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I292" s="1" t="s">
@@ -13943,7 +13943,7 @@
         <v>396</v>
       </c>
       <c r="G293" s="1" t="b">
-        <f>(B293=J293)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I293" s="1" t="s">
@@ -13979,7 +13979,7 @@
         <v>396</v>
       </c>
       <c r="G294" s="1" t="b">
-        <f>(B294=J294)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I294" s="1" t="s">
@@ -14015,7 +14015,7 @@
         <v>396</v>
       </c>
       <c r="G295" s="1" t="b">
-        <f>(B295=J295)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I295" s="1" t="s">
@@ -14051,7 +14051,7 @@
         <v>396</v>
       </c>
       <c r="G296" s="1" t="b">
-        <f>(B296=J296)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I296" s="1" t="s">
@@ -14087,7 +14087,7 @@
         <v>396</v>
       </c>
       <c r="G297" s="1" t="b">
-        <f>(B297=J297)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I297" s="1" t="s">
@@ -14123,7 +14123,7 @@
         <v>396</v>
       </c>
       <c r="G298" s="1" t="b">
-        <f>(B298=J298)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I298" s="1" t="s">
@@ -14159,7 +14159,7 @@
         <v>396</v>
       </c>
       <c r="G299" s="1" t="b">
-        <f>(B299=J299)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I299" s="1" t="s">
@@ -14195,7 +14195,7 @@
         <v>396</v>
       </c>
       <c r="G300" s="1" t="b">
-        <f>(B300=J300)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I300" s="1" t="s">
@@ -14231,7 +14231,7 @@
         <v>396</v>
       </c>
       <c r="G301" s="1" t="b">
-        <f>(B301=J301)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I301" s="1" t="s">
@@ -14267,7 +14267,7 @@
         <v>396</v>
       </c>
       <c r="G302" s="1" t="b">
-        <f>(B302=J302)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I302" s="1" t="s">
@@ -14303,7 +14303,7 @@
         <v>396</v>
       </c>
       <c r="G303" s="1" t="b">
-        <f>(B303=J303)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I303" s="1" t="s">
@@ -14339,7 +14339,7 @@
         <v>396</v>
       </c>
       <c r="G304" s="1" t="b">
-        <f>(B304=J304)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I304" s="1" t="s">
@@ -14375,7 +14375,7 @@
         <v>396</v>
       </c>
       <c r="G305" s="1" t="b">
-        <f>(B305=J305)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I305" s="1" t="s">
@@ -14411,7 +14411,7 @@
         <v>396</v>
       </c>
       <c r="G306" s="1" t="b">
-        <f>(B306=J306)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I306" s="1" t="s">
@@ -14447,7 +14447,7 @@
         <v>396</v>
       </c>
       <c r="G307" s="1" t="b">
-        <f>(B307=J307)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I307" s="1" t="s">
@@ -14483,7 +14483,7 @@
         <v>396</v>
       </c>
       <c r="G308" s="1" t="b">
-        <f>(B308=J308)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I308" s="1" t="s">
@@ -14519,7 +14519,7 @@
         <v>396</v>
       </c>
       <c r="G309" s="1" t="b">
-        <f>(B309=J309)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I309" s="1" t="s">
@@ -14555,7 +14555,7 @@
         <v>396</v>
       </c>
       <c r="G310" s="1" t="b">
-        <f>(B310=J310)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I310" s="1" t="s">
@@ -14591,7 +14591,7 @@
         <v>396</v>
       </c>
       <c r="G311" s="1" t="b">
-        <f>(B311=J311)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I311" s="1" t="s">
@@ -14627,7 +14627,7 @@
         <v>396</v>
       </c>
       <c r="G312" s="1" t="b">
-        <f>(B312=J312)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I312" s="1" t="s">
@@ -14663,7 +14663,7 @@
         <v>396</v>
       </c>
       <c r="G313" s="1" t="b">
-        <f>(B313=J313)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I313" s="1" t="s">
@@ -14699,7 +14699,7 @@
         <v>396</v>
       </c>
       <c r="G314" s="1" t="b">
-        <f>(B314=J314)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I314" s="1" t="s">
@@ -14735,7 +14735,7 @@
         <v>396</v>
       </c>
       <c r="G315" s="1" t="b">
-        <f>(B315=J315)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I315" s="1" t="s">
@@ -14771,7 +14771,7 @@
         <v>396</v>
       </c>
       <c r="G316" s="1" t="b">
-        <f>(B316=J316)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I316" s="1" t="s">
@@ -14807,7 +14807,7 @@
         <v>396</v>
       </c>
       <c r="G317" s="1" t="b">
-        <f>(B317=J317)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I317" s="1" t="s">
@@ -14843,7 +14843,7 @@
         <v>396</v>
       </c>
       <c r="G318" s="1" t="b">
-        <f>(B318=J318)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I318" s="1" t="s">
@@ -14879,7 +14879,7 @@
         <v>396</v>
       </c>
       <c r="G319" s="1" t="b">
-        <f>(B319=J319)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I319" s="1" t="s">
@@ -14915,7 +14915,7 @@
         <v>396</v>
       </c>
       <c r="G320" s="1" t="b">
-        <f>(B320=J320)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I320" s="1" t="s">
@@ -14951,7 +14951,7 @@
         <v>396</v>
       </c>
       <c r="G321" s="1" t="b">
-        <f>(B321=J321)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I321" s="1" t="s">
@@ -14987,7 +14987,7 @@
         <v>396</v>
       </c>
       <c r="G322" s="1" t="b">
-        <f>(B322=J322)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I322" s="1" t="s">
@@ -15023,7 +15023,7 @@
         <v>396</v>
       </c>
       <c r="G323" s="1" t="b">
-        <f>(B323=J323)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I323" s="1" t="s">
@@ -15059,7 +15059,7 @@
         <v>396</v>
       </c>
       <c r="G324" s="1" t="b">
-        <f>(B324=J324)</f>
+        <f t="shared" ref="G324:G387" si="5">(B324=J324)</f>
         <v>1</v>
       </c>
       <c r="I324" s="1" t="s">
@@ -15095,7 +15095,7 @@
         <v>396</v>
       </c>
       <c r="G325" s="1" t="b">
-        <f>(B325=J325)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I325" s="1" t="s">
@@ -15131,7 +15131,7 @@
         <v>396</v>
       </c>
       <c r="G326" s="1" t="b">
-        <f>(B326=J326)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I326" s="1" t="s">
@@ -15167,7 +15167,7 @@
         <v>396</v>
       </c>
       <c r="G327" s="1" t="b">
-        <f>(B327=J327)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I327" s="1" t="s">
@@ -15203,7 +15203,7 @@
         <v>396</v>
       </c>
       <c r="G328" s="1" t="b">
-        <f>(B328=J328)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I328" s="1" t="s">
@@ -15239,7 +15239,7 @@
         <v>396</v>
       </c>
       <c r="G329" s="1" t="b">
-        <f>(B329=J329)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I329" s="1" t="s">
@@ -15275,7 +15275,7 @@
         <v>8</v>
       </c>
       <c r="G330" s="1" t="b">
-        <f>(B330=J330)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I330" s="1" t="s">
@@ -15311,7 +15311,7 @@
         <v>8</v>
       </c>
       <c r="G331" s="1" t="b">
-        <f>(B331=J331)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I331" s="1" t="s">
@@ -15347,7 +15347,7 @@
         <v>8</v>
       </c>
       <c r="G332" s="1" t="b">
-        <f>(B332=J332)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I332" s="1" t="s">
@@ -15383,7 +15383,7 @@
         <v>8</v>
       </c>
       <c r="G333" s="1" t="b">
-        <f>(B333=J333)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I333" s="1" t="s">
@@ -15419,7 +15419,7 @@
         <v>8</v>
       </c>
       <c r="G334" s="1" t="b">
-        <f>(B334=J334)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I334" s="1" t="s">
@@ -15455,7 +15455,7 @@
         <v>8</v>
       </c>
       <c r="G335" s="1" t="b">
-        <f>(B335=J335)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I335" s="1" t="s">
@@ -15491,7 +15491,7 @@
         <v>8</v>
       </c>
       <c r="G336" s="1" t="b">
-        <f>(B336=J336)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I336" s="1" t="s">
@@ -15527,7 +15527,7 @@
         <v>8</v>
       </c>
       <c r="G337" s="1" t="b">
-        <f>(B337=J337)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I337" s="1" t="s">
@@ -15563,7 +15563,7 @@
         <v>8</v>
       </c>
       <c r="G338" s="1" t="b">
-        <f>(B338=J338)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I338" s="1" t="s">
@@ -15599,7 +15599,7 @@
         <v>8</v>
       </c>
       <c r="G339" s="1" t="b">
-        <f>(B339=J339)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I339" s="1" t="s">
@@ -15635,7 +15635,7 @@
         <v>8</v>
       </c>
       <c r="G340" s="1" t="b">
-        <f>(B340=J340)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I340" s="1" t="s">
@@ -15671,7 +15671,7 @@
         <v>8</v>
       </c>
       <c r="G341" s="1" t="b">
-        <f>(B341=J341)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I341" s="1" t="s">
@@ -15707,7 +15707,7 @@
         <v>8</v>
       </c>
       <c r="G342" s="1" t="b">
-        <f>(B342=J342)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I342" s="1" t="s">
@@ -15743,7 +15743,7 @@
         <v>8</v>
       </c>
       <c r="G343" s="1" t="b">
-        <f>(B343=J343)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I343" s="1" t="s">
@@ -15779,7 +15779,7 @@
         <v>8</v>
       </c>
       <c r="G344" s="1" t="b">
-        <f>(B344=J344)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I344" s="1" t="s">
@@ -15815,7 +15815,7 @@
         <v>8</v>
       </c>
       <c r="G345" s="1" t="b">
-        <f>(B345=J345)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I345" s="1" t="s">
@@ -15851,7 +15851,7 @@
         <v>8</v>
       </c>
       <c r="G346" s="1" t="b">
-        <f>(B346=J346)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I346" s="1" t="s">
@@ -15887,7 +15887,7 @@
         <v>8</v>
       </c>
       <c r="G347" s="1" t="b">
-        <f>(B347=J347)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I347" s="1" t="s">
@@ -15923,7 +15923,7 @@
         <v>8</v>
       </c>
       <c r="G348" s="1" t="b">
-        <f>(B348=J348)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I348" s="1" t="s">
@@ -15959,7 +15959,7 @@
         <v>8</v>
       </c>
       <c r="G349" s="1" t="b">
-        <f>(B349=J349)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I349" s="1" t="s">
@@ -15995,7 +15995,7 @@
         <v>8</v>
       </c>
       <c r="G350" s="1" t="b">
-        <f>(B350=J350)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I350" s="1" t="s">
@@ -16031,7 +16031,7 @@
         <v>8</v>
       </c>
       <c r="G351" s="1" t="b">
-        <f>(B351=J351)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I351" s="1" t="s">
@@ -16067,7 +16067,7 @@
         <v>8</v>
       </c>
       <c r="G352" s="1" t="b">
-        <f>(B352=J352)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I352" s="1" t="s">
@@ -16103,7 +16103,7 @@
         <v>8</v>
       </c>
       <c r="G353" s="1" t="b">
-        <f>(B353=J353)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I353" s="1" t="s">
@@ -16139,7 +16139,7 @@
         <v>8</v>
       </c>
       <c r="G354" s="1" t="b">
-        <f>(B354=J354)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I354" s="1" t="s">
@@ -16175,7 +16175,7 @@
         <v>8</v>
       </c>
       <c r="G355" s="1" t="b">
-        <f>(B355=J355)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I355" s="1" t="s">
@@ -16211,7 +16211,7 @@
         <v>8</v>
       </c>
       <c r="G356" s="1" t="b">
-        <f>(B356=J356)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I356" s="1" t="s">
@@ -16247,7 +16247,7 @@
         <v>8</v>
       </c>
       <c r="G357" s="1" t="b">
-        <f>(B357=J357)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I357" s="1" t="s">
@@ -16283,7 +16283,7 @@
         <v>8</v>
       </c>
       <c r="G358" s="1" t="b">
-        <f>(B358=J358)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I358" s="1" t="s">
@@ -16319,7 +16319,7 @@
         <v>8</v>
       </c>
       <c r="G359" s="1" t="b">
-        <f>(B359=J359)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I359" s="1" t="s">
@@ -16355,7 +16355,7 @@
         <v>8</v>
       </c>
       <c r="G360" s="1" t="b">
-        <f>(B360=J360)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I360" s="1" t="s">
@@ -16391,7 +16391,7 @@
         <v>8</v>
       </c>
       <c r="G361" s="1" t="b">
-        <f>(B361=J361)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I361" s="1" t="s">
@@ -16427,7 +16427,7 @@
         <v>8</v>
       </c>
       <c r="G362" s="1" t="b">
-        <f>(B362=J362)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I362" s="1" t="s">
@@ -16463,7 +16463,7 @@
         <v>8</v>
       </c>
       <c r="G363" s="1" t="b">
-        <f>(B363=J363)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I363" s="1" t="s">
@@ -16499,7 +16499,7 @@
         <v>8</v>
       </c>
       <c r="G364" s="1" t="b">
-        <f>(B364=J364)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I364" s="1" t="s">
@@ -16535,7 +16535,7 @@
         <v>8</v>
       </c>
       <c r="G365" s="1" t="b">
-        <f>(B365=J365)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I365" s="1" t="s">
@@ -16571,7 +16571,7 @@
         <v>8</v>
       </c>
       <c r="G366" s="1" t="b">
-        <f>(B366=J366)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I366" s="1" t="s">
@@ -16607,7 +16607,7 @@
         <v>8</v>
       </c>
       <c r="G367" s="1" t="b">
-        <f>(B367=J367)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I367" s="1" t="s">
@@ -16643,7 +16643,7 @@
         <v>8</v>
       </c>
       <c r="G368" s="1" t="b">
-        <f>(B368=J368)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I368" s="1" t="s">
@@ -16679,7 +16679,7 @@
         <v>8</v>
       </c>
       <c r="G369" s="1" t="b">
-        <f>(B369=J369)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I369" s="1" t="s">
@@ -16715,7 +16715,7 @@
         <v>8</v>
       </c>
       <c r="G370" s="1" t="b">
-        <f>(B370=J370)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I370" s="1" t="s">
@@ -16751,7 +16751,7 @@
         <v>8</v>
       </c>
       <c r="G371" s="1" t="b">
-        <f>(B371=J371)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I371" s="1" t="s">
@@ -16787,7 +16787,7 @@
         <v>8</v>
       </c>
       <c r="G372" s="1" t="b">
-        <f>(B372=J372)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I372" s="1" t="s">
@@ -16823,7 +16823,7 @@
         <v>8</v>
       </c>
       <c r="G373" s="1" t="b">
-        <f>(B373=J373)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I373" s="1" t="s">
@@ -16859,7 +16859,7 @@
         <v>8</v>
       </c>
       <c r="G374" s="1" t="b">
-        <f>(B374=J374)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I374" s="1" t="s">
@@ -16895,7 +16895,7 @@
         <v>8</v>
       </c>
       <c r="G375" s="1" t="b">
-        <f>(B375=J375)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I375" s="1" t="s">
@@ -16931,7 +16931,7 @@
         <v>8</v>
       </c>
       <c r="G376" s="1" t="b">
-        <f>(B376=J376)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I376" s="1" t="s">
@@ -16967,7 +16967,7 @@
         <v>8</v>
       </c>
       <c r="G377" s="1" t="b">
-        <f>(B377=J377)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I377" s="1" t="s">
@@ -17003,7 +17003,7 @@
         <v>8</v>
       </c>
       <c r="G378" s="1" t="b">
-        <f>(B378=J378)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I378" s="1" t="s">
@@ -17039,7 +17039,7 @@
         <v>8</v>
       </c>
       <c r="G379" s="1" t="b">
-        <f>(B379=J379)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I379" s="1" t="s">
@@ -17075,7 +17075,7 @@
         <v>8</v>
       </c>
       <c r="G380" s="1" t="b">
-        <f>(B380=J380)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I380" s="1" t="s">
@@ -17111,7 +17111,7 @@
         <v>8</v>
       </c>
       <c r="G381" s="1" t="b">
-        <f>(B381=J381)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I381" s="1" t="s">
@@ -17147,7 +17147,7 @@
         <v>8</v>
       </c>
       <c r="G382" s="1" t="b">
-        <f>(B382=J382)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I382" s="1" t="s">
@@ -17183,7 +17183,7 @@
         <v>8</v>
       </c>
       <c r="G383" s="1" t="b">
-        <f>(B383=J383)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I383" s="1" t="s">
@@ -17219,7 +17219,7 @@
         <v>8</v>
       </c>
       <c r="G384" s="1" t="b">
-        <f>(B384=J384)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I384" s="1" t="s">
@@ -17255,7 +17255,7 @@
         <v>8</v>
       </c>
       <c r="G385" s="1" t="b">
-        <f>(B385=J385)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I385" s="1" t="s">
@@ -17291,7 +17291,7 @@
         <v>8</v>
       </c>
       <c r="G386" s="1" t="b">
-        <f>(B386=J386)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I386" s="1" t="s">
@@ -17327,7 +17327,7 @@
         <v>8</v>
       </c>
       <c r="G387" s="1" t="b">
-        <f>(B387=J387)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I387" s="1" t="s">
@@ -17363,7 +17363,7 @@
         <v>8</v>
       </c>
       <c r="G388" s="1" t="b">
-        <f>(B388=J388)</f>
+        <f t="shared" ref="G388:G451" si="6">(B388=J388)</f>
         <v>1</v>
       </c>
       <c r="I388" s="1" t="s">
@@ -17399,7 +17399,7 @@
         <v>8</v>
       </c>
       <c r="G389" s="1" t="b">
-        <f>(B389=J389)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I389" s="1" t="s">
@@ -17435,7 +17435,7 @@
         <v>8</v>
       </c>
       <c r="G390" s="1" t="b">
-        <f>(B390=J390)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I390" s="1" t="s">
@@ -17471,7 +17471,7 @@
         <v>8</v>
       </c>
       <c r="G391" s="1" t="b">
-        <f>(B391=J391)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I391" s="1" t="s">
@@ -17507,7 +17507,7 @@
         <v>8</v>
       </c>
       <c r="G392" s="1" t="b">
-        <f>(B392=J392)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I392" s="1" t="s">
@@ -17543,7 +17543,7 @@
         <v>8</v>
       </c>
       <c r="G393" s="1" t="b">
-        <f>(B393=J393)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I393" s="1" t="s">
@@ -17579,7 +17579,7 @@
         <v>8</v>
       </c>
       <c r="G394" s="1" t="b">
-        <f>(B394=J394)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I394" s="1" t="s">
@@ -17615,7 +17615,7 @@
         <v>8</v>
       </c>
       <c r="G395" s="1" t="b">
-        <f>(B395=J395)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I395" s="1" t="s">
@@ -17651,7 +17651,7 @@
         <v>8</v>
       </c>
       <c r="G396" s="1" t="b">
-        <f>(B396=J396)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I396" s="1" t="s">
@@ -17687,7 +17687,7 @@
         <v>8</v>
       </c>
       <c r="G397" s="1" t="b">
-        <f>(B397=J397)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I397" s="1" t="s">
@@ -17723,7 +17723,7 @@
         <v>8</v>
       </c>
       <c r="G398" s="1" t="b">
-        <f>(B398=J398)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I398" s="1" t="s">
@@ -17759,7 +17759,7 @@
         <v>8</v>
       </c>
       <c r="G399" s="1" t="b">
-        <f>(B399=J399)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I399" s="1" t="s">
@@ -17795,7 +17795,7 @@
         <v>8</v>
       </c>
       <c r="G400" s="1" t="b">
-        <f>(B400=J400)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I400" s="1" t="s">
@@ -17831,7 +17831,7 @@
         <v>8</v>
       </c>
       <c r="G401" s="1" t="b">
-        <f>(B401=J401)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I401" s="1" t="s">
@@ -17867,7 +17867,7 @@
         <v>8</v>
       </c>
       <c r="G402" s="1" t="b">
-        <f>(B402=J402)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I402" s="1" t="s">
@@ -17903,7 +17903,7 @@
         <v>8</v>
       </c>
       <c r="G403" s="1" t="b">
-        <f>(B403=J403)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I403" s="1" t="s">
@@ -17939,7 +17939,7 @@
         <v>8</v>
       </c>
       <c r="G404" s="1" t="b">
-        <f>(B404=J404)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I404" s="1" t="s">
@@ -17975,7 +17975,7 @@
         <v>8</v>
       </c>
       <c r="G405" s="1" t="b">
-        <f>(B405=J405)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I405" s="1" t="s">
@@ -18011,7 +18011,7 @@
         <v>8</v>
       </c>
       <c r="G406" s="1" t="b">
-        <f>(B406=J406)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I406" s="1" t="s">
@@ -18047,7 +18047,7 @@
         <v>8</v>
       </c>
       <c r="G407" s="1" t="b">
-        <f>(B407=J407)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I407" s="1" t="s">
@@ -18083,7 +18083,7 @@
         <v>8</v>
       </c>
       <c r="G408" s="1" t="b">
-        <f>(B408=J408)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I408" s="1" t="s">
@@ -18119,7 +18119,7 @@
         <v>8</v>
       </c>
       <c r="G409" s="1" t="b">
-        <f>(B409=J409)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I409" s="1" t="s">
@@ -18155,7 +18155,7 @@
         <v>8</v>
       </c>
       <c r="G410" s="1" t="b">
-        <f>(B410=J410)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I410" s="1" t="s">
@@ -18191,7 +18191,7 @@
         <v>8</v>
       </c>
       <c r="G411" s="1" t="b">
-        <f>(B411=J411)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I411" s="1" t="s">
@@ -18227,7 +18227,7 @@
         <v>8</v>
       </c>
       <c r="G412" s="1" t="b">
-        <f>(B412=J412)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I412" s="1" t="s">
@@ -18263,7 +18263,7 @@
         <v>8</v>
       </c>
       <c r="G413" s="1" t="b">
-        <f>(B413=J413)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I413" s="1" t="s">
@@ -18299,7 +18299,7 @@
         <v>8</v>
       </c>
       <c r="G414" s="1" t="b">
-        <f>(B414=J414)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I414" s="1" t="s">
@@ -18335,7 +18335,7 @@
         <v>8</v>
       </c>
       <c r="G415" s="1" t="b">
-        <f>(B415=J415)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I415" s="1" t="s">
@@ -18371,7 +18371,7 @@
         <v>8</v>
       </c>
       <c r="G416" s="1" t="b">
-        <f>(B416=J416)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I416" s="1" t="s">
@@ -18407,7 +18407,7 @@
         <v>8</v>
       </c>
       <c r="G417" s="1" t="b">
-        <f>(B417=J417)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I417" s="1" t="s">
@@ -18443,7 +18443,7 @@
         <v>8</v>
       </c>
       <c r="G418" s="1" t="b">
-        <f>(B418=J418)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I418" s="1" t="s">
@@ -18479,7 +18479,7 @@
         <v>8</v>
       </c>
       <c r="G419" s="1" t="b">
-        <f>(B419=J419)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I419" s="1" t="s">
@@ -18515,7 +18515,7 @@
         <v>8</v>
       </c>
       <c r="G420" s="1" t="b">
-        <f>(B420=J420)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I420" s="1" t="s">
@@ -18551,7 +18551,7 @@
         <v>8</v>
       </c>
       <c r="G421" s="1" t="b">
-        <f>(B421=J421)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I421" s="1" t="s">
@@ -18587,7 +18587,7 @@
         <v>8</v>
       </c>
       <c r="G422" s="1" t="b">
-        <f>(B422=J422)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I422" s="1" t="s">
@@ -18623,7 +18623,7 @@
         <v>8</v>
       </c>
       <c r="G423" s="1" t="b">
-        <f>(B423=J423)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I423" s="1" t="s">
@@ -18659,7 +18659,7 @@
         <v>8</v>
       </c>
       <c r="G424" s="1" t="b">
-        <f>(B424=J424)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I424" s="1" t="s">
@@ -18695,7 +18695,7 @@
         <v>8</v>
       </c>
       <c r="G425" s="1" t="b">
-        <f>(B425=J425)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I425" s="1" t="s">
@@ -18731,7 +18731,7 @@
         <v>8</v>
       </c>
       <c r="G426" s="1" t="b">
-        <f>(B426=J426)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I426" s="1" t="s">
@@ -18767,7 +18767,7 @@
         <v>8</v>
       </c>
       <c r="G427" s="1" t="b">
-        <f>(B427=J427)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I427" s="1" t="s">
@@ -18803,7 +18803,7 @@
         <v>8</v>
       </c>
       <c r="G428" s="1" t="b">
-        <f>(B428=J428)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I428" s="1" t="s">
@@ -18839,7 +18839,7 @@
         <v>8</v>
       </c>
       <c r="G429" s="1" t="b">
-        <f>(B429=J429)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I429" s="1" t="s">
@@ -18875,7 +18875,7 @@
         <v>8</v>
       </c>
       <c r="G430" s="1" t="b">
-        <f>(B430=J430)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I430" s="1" t="s">
@@ -18911,7 +18911,7 @@
         <v>8</v>
       </c>
       <c r="G431" s="1" t="b">
-        <f>(B431=J431)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I431" s="1" t="s">
@@ -18947,7 +18947,7 @@
         <v>8</v>
       </c>
       <c r="G432" s="1" t="b">
-        <f>(B432=J432)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I432" s="1" t="s">
@@ -18983,7 +18983,7 @@
         <v>8</v>
       </c>
       <c r="G433" s="1" t="b">
-        <f>(B433=J433)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I433" s="1" t="s">
@@ -19019,7 +19019,7 @@
         <v>8</v>
       </c>
       <c r="G434" s="1" t="b">
-        <f>(B434=J434)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I434" s="1" t="s">
@@ -19055,7 +19055,7 @@
         <v>8</v>
       </c>
       <c r="G435" s="1" t="b">
-        <f>(B435=J435)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I435" s="1" t="s">
@@ -19091,7 +19091,7 @@
         <v>8</v>
       </c>
       <c r="G436" s="1" t="b">
-        <f>(B436=J436)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I436" s="1" t="s">
@@ -19127,7 +19127,7 @@
         <v>8</v>
       </c>
       <c r="G437" s="1" t="b">
-        <f>(B437=J437)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I437" s="1" t="s">
@@ -19163,7 +19163,7 @@
         <v>8</v>
       </c>
       <c r="G438" s="1" t="b">
-        <f>(B438=J438)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I438" s="1" t="s">
@@ -19199,7 +19199,7 @@
         <v>8</v>
       </c>
       <c r="G439" s="1" t="b">
-        <f>(B439=J439)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I439" s="1" t="s">
@@ -19235,7 +19235,7 @@
         <v>8</v>
       </c>
       <c r="G440" s="1" t="b">
-        <f>(B440=J440)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I440" s="1" t="s">
@@ -19271,7 +19271,7 @@
         <v>8</v>
       </c>
       <c r="G441" s="1" t="b">
-        <f>(B441=J441)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I441" s="1" t="s">
@@ -19307,7 +19307,7 @@
         <v>8</v>
       </c>
       <c r="G442" s="1" t="b">
-        <f>(B442=J442)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I442" s="1" t="s">
@@ -19343,7 +19343,7 @@
         <v>8</v>
       </c>
       <c r="G443" s="1" t="b">
-        <f>(B443=J443)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I443" s="1" t="s">
@@ -19379,7 +19379,7 @@
         <v>8</v>
       </c>
       <c r="G444" s="1" t="b">
-        <f>(B444=J444)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I444" s="1" t="s">
@@ -19415,7 +19415,7 @@
         <v>8</v>
       </c>
       <c r="G445" s="1" t="b">
-        <f>(B445=J445)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I445" s="1" t="s">
@@ -19451,7 +19451,7 @@
         <v>8</v>
       </c>
       <c r="G446" s="1" t="b">
-        <f>(B446=J446)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I446" s="1" t="s">
@@ -19487,7 +19487,7 @@
         <v>8</v>
       </c>
       <c r="G447" s="1" t="b">
-        <f>(B447=J447)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I447" s="1" t="s">
@@ -19523,7 +19523,7 @@
         <v>8</v>
       </c>
       <c r="G448" s="1" t="b">
-        <f>(B448=J448)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I448" s="1" t="s">
@@ -19559,7 +19559,7 @@
         <v>8</v>
       </c>
       <c r="G449" s="1" t="b">
-        <f>(B449=J449)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I449" s="1" t="s">
@@ -19595,7 +19595,7 @@
         <v>8</v>
       </c>
       <c r="G450" s="1" t="b">
-        <f>(B450=J450)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I450" s="1" t="s">
@@ -19631,7 +19631,7 @@
         <v>8</v>
       </c>
       <c r="G451" s="1" t="b">
-        <f>(B451=J451)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I451" s="1" t="s">
@@ -19667,7 +19667,7 @@
         <v>8</v>
       </c>
       <c r="G452" s="1" t="b">
-        <f>(B452=J452)</f>
+        <f t="shared" ref="G452:G487" si="7">(B452=J452)</f>
         <v>1</v>
       </c>
       <c r="I452" s="1" t="s">
@@ -19703,7 +19703,7 @@
         <v>8</v>
       </c>
       <c r="G453" s="1" t="b">
-        <f>(B453=J453)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I453" s="1" t="s">
@@ -19739,7 +19739,7 @@
         <v>8</v>
       </c>
       <c r="G454" s="1" t="b">
-        <f>(B454=J454)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I454" s="1" t="s">
@@ -19775,7 +19775,7 @@
         <v>8</v>
       </c>
       <c r="G455" s="1" t="b">
-        <f>(B455=J455)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I455" s="1" t="s">
@@ -19811,7 +19811,7 @@
         <v>8</v>
       </c>
       <c r="G456" s="1" t="b">
-        <f>(B456=J456)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I456" s="1" t="s">
@@ -19847,7 +19847,7 @@
         <v>8</v>
       </c>
       <c r="G457" s="1" t="b">
-        <f>(B457=J457)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I457" s="1" t="s">
@@ -19883,7 +19883,7 @@
         <v>8</v>
       </c>
       <c r="G458" s="1" t="b">
-        <f>(B458=J458)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I458" s="1" t="s">
@@ -19919,7 +19919,7 @@
         <v>8</v>
       </c>
       <c r="G459" s="1" t="b">
-        <f>(B459=J459)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I459" s="1" t="s">
@@ -19955,7 +19955,7 @@
         <v>8</v>
       </c>
       <c r="G460" s="1" t="b">
-        <f>(B460=J460)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I460" s="1" t="s">
@@ -19992,7 +19992,7 @@
       </c>
       <c r="F461" s="2"/>
       <c r="G461" s="2" t="b">
-        <f>(B461=J461)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H461" s="2"/>
@@ -20029,7 +20029,7 @@
         <v>8</v>
       </c>
       <c r="G462" s="1" t="b">
-        <f>(B462=J462)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I462" s="1" t="s">
@@ -20065,7 +20065,7 @@
         <v>8</v>
       </c>
       <c r="G463" s="1" t="b">
-        <f>(B463=J463)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I463" s="1" t="s">
@@ -20101,7 +20101,7 @@
         <v>8</v>
       </c>
       <c r="G464" s="1" t="b">
-        <f>(B464=J464)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I464" s="1" t="s">
@@ -20137,7 +20137,7 @@
         <v>8</v>
       </c>
       <c r="G465" s="1" t="b">
-        <f>(B465=J465)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I465" s="1" t="s">
@@ -20173,7 +20173,7 @@
         <v>8</v>
       </c>
       <c r="G466" s="1" t="b">
-        <f>(B466=J466)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I466" s="1" t="s">
@@ -20209,7 +20209,7 @@
         <v>8</v>
       </c>
       <c r="G467" s="1" t="b">
-        <f>(B467=J467)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I467" s="1" t="s">
@@ -20245,7 +20245,7 @@
         <v>8</v>
       </c>
       <c r="G468" s="1" t="b">
-        <f>(B468=J468)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I468" s="1" t="s">
@@ -20281,7 +20281,7 @@
         <v>8</v>
       </c>
       <c r="G469" s="1" t="b">
-        <f>(B469=J469)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I469" s="1" t="s">
@@ -20317,7 +20317,7 @@
         <v>8</v>
       </c>
       <c r="G470" s="1" t="b">
-        <f>(B470=J470)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I470" s="1" t="s">
@@ -20353,7 +20353,7 @@
         <v>8</v>
       </c>
       <c r="G471" s="1" t="b">
-        <f>(B471=J471)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I471" s="1" t="s">
@@ -20389,7 +20389,7 @@
         <v>8</v>
       </c>
       <c r="G472" s="1" t="b">
-        <f>(B472=J472)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I472" s="1" t="s">
@@ -20425,7 +20425,7 @@
         <v>8</v>
       </c>
       <c r="G473" s="1" t="b">
-        <f>(B473=J473)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I473" s="1" t="s">
@@ -20461,7 +20461,7 @@
         <v>8</v>
       </c>
       <c r="G474" s="1" t="b">
-        <f>(B474=J474)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I474" s="1" t="s">
@@ -20497,7 +20497,7 @@
         <v>8</v>
       </c>
       <c r="G475" s="1" t="b">
-        <f>(B475=J475)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I475" s="1" t="s">
@@ -20533,7 +20533,7 @@
         <v>8</v>
       </c>
       <c r="G476" s="1" t="b">
-        <f>(B476=J476)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I476" s="1" t="s">
@@ -20569,7 +20569,7 @@
         <v>8</v>
       </c>
       <c r="G477" s="1" t="b">
-        <f>(B477=J477)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I477" s="1" t="s">
@@ -20605,7 +20605,7 @@
         <v>8</v>
       </c>
       <c r="G478" s="1" t="b">
-        <f>(B478=J478)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I478" s="1" t="s">
@@ -20641,7 +20641,7 @@
         <v>8</v>
       </c>
       <c r="G479" s="1" t="b">
-        <f>(B479=J479)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I479" s="1" t="s">
@@ -20677,7 +20677,7 @@
         <v>8</v>
       </c>
       <c r="G480" s="1" t="b">
-        <f>(B480=J480)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I480" s="1" t="s">
@@ -20713,7 +20713,7 @@
         <v>8</v>
       </c>
       <c r="G481" s="1" t="b">
-        <f>(B481=J481)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I481" s="1" t="s">
@@ -20749,7 +20749,7 @@
         <v>8</v>
       </c>
       <c r="G482" s="1" t="b">
-        <f>(B482=J482)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I482" s="1" t="s">
@@ -20785,7 +20785,7 @@
         <v>8</v>
       </c>
       <c r="G483" s="1" t="b">
-        <f>(B483=J483)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I483" s="1" t="s">
@@ -20821,7 +20821,7 @@
         <v>8</v>
       </c>
       <c r="G484" s="1" t="b">
-        <f>(B484=J484)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I484" s="1" t="s">
@@ -20857,7 +20857,7 @@
         <v>8</v>
       </c>
       <c r="G485" s="1" t="b">
-        <f>(B485=J485)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I485" s="1" t="s">
@@ -20893,7 +20893,7 @@
         <v>8</v>
       </c>
       <c r="G486" s="1" t="b">
-        <f>(B486=J486)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I486" s="1" t="s">
@@ -20929,7 +20929,7 @@
         <v>8</v>
       </c>
       <c r="G487" s="1" t="b">
-        <f>(B487=J487)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I487" s="1" t="s">

</xml_diff>